<commit_message>
[swobup test] fix Table name
</commit_message>
<xml_diff>
--- a/templates/dataplant/test_dominik.xlsx
+++ b/templates/dataplant/test_dominik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33E8DB60-7182-9745-86AD-F045218955FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F761E5D-81ED-0A41-AD94-C22C945621D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13400" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{12DA3DB9-A0DA-2649-9EF0-DEFE326F12C7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Source Name</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>1.0.0</t>
+  </si>
+  <si>
+    <t>annotationTablePrettyGecko11</t>
   </si>
 </sst>
 </file>
@@ -695,7 +698,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,7 +754,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,7 +803,9 @@
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">

</xml_diff>